<commit_message>
Processors: x86: AMD: Update
</commit_message>
<xml_diff>
--- a/Processors/Performance/Benchmarks.xlsx
+++ b/Processors/Performance/Benchmarks.xlsx
@@ -9,7 +9,7 @@
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="34">
   <si>
     <t>CPU</t>
   </si>
@@ -146,6 +146,18 @@
   </si>
   <si>
     <t>Cores</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>7945HX</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>8700G</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>i5-14600K</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -473,11 +485,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H25"/>
+  <dimension ref="A1:H28"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="J10" sqref="J10"/>
+      <selection pane="bottomLeft" activeCell="H11" sqref="H11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -530,7 +542,7 @@
         <v>4733</v>
       </c>
       <c r="E2">
-        <f t="shared" ref="E2:E18" si="0">D2/C2</f>
+        <f t="shared" ref="E2:E21" si="0">D2/C2</f>
         <v>1.3522857142857143</v>
       </c>
       <c r="F2">
@@ -603,7 +615,7 @@
         <v>37065</v>
       </c>
       <c r="G5">
-        <f t="shared" ref="G5:G15" si="1">F5/D5</f>
+        <f t="shared" ref="G5:G19" si="1">F5/D5</f>
         <v>7.9709677419354836</v>
       </c>
       <c r="H5">
@@ -642,272 +654,309 @@
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="B7" s="2">
+        <v>12</v>
+      </c>
+      <c r="C7">
+        <v>1450</v>
+      </c>
+      <c r="D7">
+        <v>3944</v>
+      </c>
+      <c r="E7">
+        <f>D7/C7</f>
+        <v>2.72</v>
+      </c>
+      <c r="F7">
+        <v>31797</v>
+      </c>
+      <c r="G7">
+        <f t="shared" si="1"/>
+        <v>8.0621196754563886</v>
+      </c>
+      <c r="H7">
+        <f>F7/C7</f>
+        <v>21.92896551724138</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A8" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="B7" s="2">
-        <v>2</v>
-      </c>
-      <c r="C7">
+      <c r="B8" s="2">
+        <v>2</v>
+      </c>
+      <c r="C8">
         <v>2600</v>
       </c>
-      <c r="D7">
+      <c r="D8">
         <v>4275</v>
       </c>
-      <c r="E7">
+      <c r="E8">
         <f t="shared" si="0"/>
         <v>1.6442307692307692</v>
       </c>
-      <c r="F7">
+      <c r="F8">
         <v>62682</v>
       </c>
-      <c r="G7">
+      <c r="G8">
         <f t="shared" si="1"/>
         <v>14.662456140350876</v>
       </c>
-      <c r="H7">
-        <f>F7/C7</f>
+      <c r="H8">
+        <f>F8/C8</f>
         <v>24.108461538461537</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A8" s="1" t="s">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A9" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="B8" s="2">
-        <v>2</v>
-      </c>
-      <c r="C8">
+      <c r="B9" s="2">
+        <v>2</v>
+      </c>
+      <c r="C9">
         <v>3600</v>
       </c>
-      <c r="D8">
+      <c r="D9">
         <v>4150</v>
       </c>
-      <c r="E8">
-        <f>D8/C8</f>
+      <c r="E9">
+        <f>D9/C9</f>
         <v>1.1527777777777777</v>
       </c>
-      <c r="F8">
+      <c r="F9">
         <v>62507</v>
       </c>
-      <c r="G8">
+      <c r="G9">
         <f t="shared" si="1"/>
         <v>15.061927710843374</v>
       </c>
-      <c r="H8">
-        <f>F8/C8</f>
+      <c r="H9">
+        <f>F9/C9</f>
         <v>17.363055555555555</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A9" s="1" t="s">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A10" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="B10" s="2"/>
+      <c r="D10">
+        <v>4049</v>
+      </c>
+      <c r="F10">
+        <v>54682</v>
+      </c>
+      <c r="G10">
+        <f t="shared" si="1"/>
+        <v>13.505062978513212</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A11" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="B9" s="2">
-        <v>2</v>
-      </c>
-      <c r="C9">
+      <c r="B11" s="2">
+        <v>2</v>
+      </c>
+      <c r="C11">
         <v>1800</v>
       </c>
-      <c r="D9">
+      <c r="D11">
         <v>4251</v>
       </c>
-      <c r="E9">
+      <c r="E11">
         <f t="shared" si="0"/>
         <v>2.3616666666666668</v>
       </c>
-      <c r="F9">
+      <c r="F11">
         <v>51639</v>
       </c>
-      <c r="G9">
+      <c r="G11">
         <f t="shared" si="1"/>
         <v>12.147494707127734</v>
       </c>
-      <c r="H9">
-        <f>F9/C9</f>
+      <c r="H11">
+        <f>F11/C11</f>
         <v>28.688333333333333</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A10" s="1" t="s">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A12" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="B10" s="2">
-        <v>2</v>
-      </c>
-      <c r="F10">
+      <c r="B12" s="2">
+        <v>2</v>
+      </c>
+      <c r="F12">
         <v>50411</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A11" s="1" t="s">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A13" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="B11" s="2">
-        <v>2</v>
-      </c>
-      <c r="C11">
+      <c r="B13" s="2">
+        <v>2</v>
+      </c>
+      <c r="C13">
         <v>1750</v>
       </c>
-      <c r="D11">
+      <c r="D13">
         <v>4147</v>
       </c>
-      <c r="F11">
+      <c r="F13">
         <v>48781</v>
       </c>
-      <c r="G11">
+      <c r="G13">
         <f t="shared" si="1"/>
         <v>11.762961176754279</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A12" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="B12" s="2"/>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A13" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="B13" s="2">
-        <v>2</v>
-      </c>
-      <c r="C13">
-        <v>1450</v>
-      </c>
-      <c r="F13">
-        <v>35955</v>
-      </c>
-      <c r="H13">
-        <f>F13/C13</f>
-        <v>24.796551724137931</v>
-      </c>
-    </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A14" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="B14" s="2">
-        <v>2</v>
-      </c>
-      <c r="C14">
-        <v>1200</v>
-      </c>
+        <v>26</v>
+      </c>
+      <c r="B14" s="2"/>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A15" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B15" s="2">
+        <v>2</v>
+      </c>
+      <c r="C15">
+        <v>1450</v>
+      </c>
+      <c r="F15">
+        <v>35955</v>
+      </c>
+      <c r="H15">
+        <f>F15/C15</f>
+        <v>24.796551724137931</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A16" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="B16" s="2">
+        <v>2</v>
+      </c>
+      <c r="C16">
+        <v>1200</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A17" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="B15" s="2">
-        <v>2</v>
-      </c>
-      <c r="C15">
+      <c r="B17" s="2">
+        <v>2</v>
+      </c>
+      <c r="C17">
         <v>1000</v>
       </c>
-      <c r="D15">
+      <c r="D17">
         <v>4145</v>
       </c>
-      <c r="E15">
-        <f>D15/C15</f>
+      <c r="E17">
+        <f>D17/C17</f>
         <v>4.1449999999999996</v>
       </c>
-      <c r="F15">
+      <c r="F17">
         <v>28476</v>
       </c>
-      <c r="G15">
+      <c r="G17">
         <f t="shared" si="1"/>
         <v>6.8699638118214716</v>
       </c>
-      <c r="H15">
-        <f>F15/C15</f>
-        <v>28.475999999999999</v>
-      </c>
-    </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A16" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="B16" s="2">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A17" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="B17" s="2">
-        <v>0</v>
-      </c>
-      <c r="C17">
-        <v>700</v>
-      </c>
-      <c r="D17">
-        <v>3902</v>
-      </c>
-      <c r="E17">
-        <f>D17/C17</f>
-        <v>5.5742857142857138</v>
-      </c>
-      <c r="F17">
-        <v>27574</v>
-      </c>
       <c r="H17">
         <f>F17/C17</f>
-        <v>39.39142857142857</v>
+        <v>28.475999999999999</v>
       </c>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A18" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="B18" s="2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A19" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="B19" s="2"/>
+      <c r="D19">
+        <v>4285</v>
+      </c>
+      <c r="F19">
+        <v>38830</v>
+      </c>
+      <c r="G19">
+        <f t="shared" si="1"/>
+        <v>9.0618436406067673</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A20" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B20" s="2">
+        <v>0</v>
+      </c>
+      <c r="C20">
+        <v>700</v>
+      </c>
+      <c r="D20">
+        <v>3902</v>
+      </c>
+      <c r="E20">
+        <f>D20/C20</f>
+        <v>5.5742857142857138</v>
+      </c>
+      <c r="F20">
+        <v>27574</v>
+      </c>
+      <c r="H20">
+        <f>F20/C20</f>
+        <v>39.39142857142857</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A21" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B18" s="2">
+      <c r="B21" s="2">
         <v>0</v>
       </c>
-      <c r="C18">
+      <c r="C21">
         <v>1800</v>
       </c>
-      <c r="D18">
+      <c r="D21">
         <v>3470</v>
       </c>
-      <c r="E18">
+      <c r="E21">
         <f t="shared" si="0"/>
         <v>1.9277777777777778</v>
       </c>
-      <c r="F18">
+      <c r="F21">
         <v>45597</v>
       </c>
-      <c r="H18">
-        <f>F18/C18</f>
+      <c r="H21">
+        <f>F21/C21</f>
         <v>25.331666666666667</v>
-      </c>
-    </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A19" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="B19" s="2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A20" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="B20" s="2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A21" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="B21" s="2">
-        <v>0</v>
       </c>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A22" s="1" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="B22" s="2">
         <v>0</v>
@@ -915,7 +964,7 @@
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A23" s="1" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B23" s="2">
         <v>0</v>
@@ -923,47 +972,71 @@
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A24" s="1" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="B24" s="2">
-        <v>12</v>
-      </c>
-      <c r="D24">
-        <v>3286</v>
-      </c>
-      <c r="F24">
-        <v>23566</v>
+        <v>0</v>
       </c>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A25" s="1">
-        <v>3600</v>
+      <c r="A25" s="1" t="s">
+        <v>16</v>
       </c>
       <c r="B25" s="2">
         <v>0</v>
       </c>
-      <c r="C25">
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A26" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B26" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A27" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B27" s="2">
+        <v>12</v>
+      </c>
+      <c r="D27">
+        <v>3286</v>
+      </c>
+      <c r="F27">
+        <v>23566</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A28" s="1">
+        <v>3600</v>
+      </c>
+      <c r="B28" s="2">
+        <v>0</v>
+      </c>
+      <c r="C28">
         <v>230</v>
       </c>
-      <c r="D25">
+      <c r="D28">
         <v>2566</v>
       </c>
-      <c r="E25">
-        <f>D25/C25</f>
+      <c r="E28">
+        <f>D28/C28</f>
         <v>11.156521739130435</v>
       </c>
-      <c r="F25">
+      <c r="F28">
         <v>17742</v>
       </c>
-      <c r="H25">
-        <f>F25/C25</f>
+      <c r="H28">
+        <f>F28/C28</f>
         <v>77.139130434782615</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <conditionalFormatting sqref="C1:C1048576 F1:G1048576">
-    <cfRule type="colorScale" priority="6">
+    <cfRule type="colorScale" priority="7">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="max"/>
@@ -972,7 +1045,17 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D17:D1048576 D15 D1:D9 D11:D13 H1:H1048576">
+  <conditionalFormatting sqref="D20:D1048576 D17 D1:D11 D13:D15 H1:H1048576">
+    <cfRule type="colorScale" priority="10">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FFFFEF9C"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E1:E1048576">
     <cfRule type="colorScale" priority="9">
       <colorScale>
         <cfvo type="min"/>
@@ -982,8 +1065,8 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E1:E1048576">
-    <cfRule type="colorScale" priority="8">
+  <conditionalFormatting sqref="B1:B1048576">
+    <cfRule type="colorScale" priority="2">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="max"/>
@@ -992,7 +1075,37 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B1:B1048576">
+  <conditionalFormatting sqref="H1:H1048576">
+    <cfRule type="colorScale" priority="6">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FFFFEF9C"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F1:G1048576">
+    <cfRule type="colorScale" priority="5">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FFFFEF9C"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D20:D1048576 D17 D1:D11 D13:D15">
+    <cfRule type="colorScale" priority="4">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FFFFEF9C"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D1:D1048576">
     <cfRule type="colorScale" priority="1">
       <colorScale>
         <cfvo type="min"/>
@@ -1002,37 +1115,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H1:H1048576">
-    <cfRule type="colorScale" priority="5">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="max"/>
-        <color rgb="FFFFEF9C"/>
-        <color rgb="FF63BE7B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="F1:G1048576">
-    <cfRule type="colorScale" priority="4">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="max"/>
-        <color rgb="FFFFEF9C"/>
-        <color rgb="FF63BE7B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D17:D1048576 D15 D1:D9 D11:D13">
-    <cfRule type="colorScale" priority="3">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="max"/>
-        <color rgb="FFFFEF9C"/>
-        <color rgb="FF63BE7B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>